<commit_message>
Make changes in the excel with the data and in the script make module to write for more than one timeslice the parameter SpecifiedProfileDemand
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Outputs/A-O_Demand.xlsx
+++ b/t1_confection/A1_Outputs/A-O_Demand.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisfernando\Dropbox\2_WORK\MOMF\RD_Model_v9_clean_new\A1_Outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t1_confection\A1_Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303696FF-3226-44B4-B338-F5CC94F5BAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0DABE5-3865-424E-B0CA-4F2027C862BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Demand_Projection" sheetId="1" r:id="rId1"/>
+    <sheet name="Timeslices" sheetId="3" r:id="rId1"/>
+    <sheet name="Demand_Projection" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -351,7 +352,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="169">
   <si>
     <t>Demand/Share</t>
   </si>
@@ -849,6 +850,15 @@
   </si>
   <si>
     <t>Transport Demand non motorized reductions</t>
+  </si>
+  <si>
+    <t>Timeslice</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1530,6 +1540,7 @@
     <xf numFmtId="166" fontId="6" fillId="13" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1854,29 +1865,699 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037C0E4B-223C-493A-AA95-0D314598A9DF}">
+  <dimension ref="A1:AP5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A1" s="91" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2023</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2024</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2026</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2027</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2028</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2029</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2030</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2031</v>
+      </c>
+      <c r="X1" s="1">
+        <v>2032</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>2033</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>2034</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>2035</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>2036</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>2037</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>2038</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>2039</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>2040</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>2041</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>2042</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>2043</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>2044</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>2045</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>2046</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>2047</v>
+      </c>
+      <c r="AN1" s="1">
+        <v>2048</v>
+      </c>
+      <c r="AO1" s="1">
+        <v>2049</v>
+      </c>
+      <c r="AP1" s="1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1.130436</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1.3405151997302078</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1.155981494838745</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1.3158819494067027</v>
+      </c>
+      <c r="N2" s="20">
+        <v>1.228027468725523</v>
+      </c>
+      <c r="O2" s="20">
+        <v>1.2225466516920374</v>
+      </c>
+      <c r="P2" s="20">
+        <v>1.2642991758160602</v>
+      </c>
+      <c r="Q2" s="20">
+        <v>1.3061603371669015</v>
+      </c>
+      <c r="R2" s="20">
+        <v>1.3457029459936605</v>
+      </c>
+      <c r="S2" s="20">
+        <v>1.385820995226948</v>
+      </c>
+      <c r="T2" s="20">
+        <v>1.4283570465266955</v>
+      </c>
+      <c r="U2" s="20">
+        <v>1.4693026793705557</v>
+      </c>
+      <c r="V2" s="20">
+        <v>1.5100626733919791</v>
+      </c>
+      <c r="W2" s="20">
+        <v>1.5470140015439409</v>
+      </c>
+      <c r="X2" s="20">
+        <v>1.5846567014175537</v>
+      </c>
+      <c r="Y2" s="20">
+        <v>1.6229997712220672</v>
+      </c>
+      <c r="Z2" s="20">
+        <v>1.6620522756006084</v>
+      </c>
+      <c r="AA2" s="20">
+        <v>1.70182334575065</v>
+      </c>
+      <c r="AB2" s="20">
+        <v>1.7353881862675751</v>
+      </c>
+      <c r="AC2" s="20">
+        <v>1.7694597550384985</v>
+      </c>
+      <c r="AD2" s="20">
+        <v>1.804043379247714</v>
+      </c>
+      <c r="AE2" s="20">
+        <v>1.8391444178829401</v>
+      </c>
+      <c r="AF2" s="20">
+        <v>1.8747682617819925</v>
+      </c>
+      <c r="AG2" s="20">
+        <v>1.9037214287348594</v>
+      </c>
+      <c r="AH2" s="20">
+        <v>1.9330171998608836</v>
+      </c>
+      <c r="AI2" s="20">
+        <v>1.9626584009867136</v>
+      </c>
+      <c r="AJ2" s="20">
+        <v>1.9926478711876765</v>
+      </c>
+      <c r="AK2" s="20">
+        <v>2.0229884628030699</v>
+      </c>
+      <c r="AL2" s="20">
+        <v>2.0465590535637337</v>
+      </c>
+      <c r="AM2" s="20">
+        <v>2.0703402523753147</v>
+      </c>
+      <c r="AN2" s="20">
+        <v>2.0943333720806838</v>
+      </c>
+      <c r="AO2" s="20">
+        <v>2.1185397301785733</v>
+      </c>
+      <c r="AP2" s="20">
+        <v>2.1429606488276343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.130436</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1.3405151997302078</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1.155981494838745</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1.3158819494067027</v>
+      </c>
+      <c r="N3" s="20">
+        <v>1.228027468725523</v>
+      </c>
+      <c r="O3" s="20">
+        <v>1.2225466516920374</v>
+      </c>
+      <c r="P3" s="20">
+        <v>1.2642991758160602</v>
+      </c>
+      <c r="Q3" s="20">
+        <v>1.3061603371669015</v>
+      </c>
+      <c r="R3" s="20">
+        <v>1.3457029459936605</v>
+      </c>
+      <c r="S3" s="20">
+        <v>1.385820995226948</v>
+      </c>
+      <c r="T3" s="20">
+        <v>1.4283570465266955</v>
+      </c>
+      <c r="U3" s="20">
+        <v>1.4693026793705557</v>
+      </c>
+      <c r="V3" s="20">
+        <v>1.5100626733919791</v>
+      </c>
+      <c r="W3" s="20">
+        <v>1.5470140015439409</v>
+      </c>
+      <c r="X3" s="20">
+        <v>1.5846567014175537</v>
+      </c>
+      <c r="Y3" s="20">
+        <v>1.6229997712220672</v>
+      </c>
+      <c r="Z3" s="20">
+        <v>1.6620522756006084</v>
+      </c>
+      <c r="AA3" s="20">
+        <v>1.70182334575065</v>
+      </c>
+      <c r="AB3" s="20">
+        <v>1.7353881862675751</v>
+      </c>
+      <c r="AC3" s="20">
+        <v>1.7694597550384985</v>
+      </c>
+      <c r="AD3" s="20">
+        <v>1.804043379247714</v>
+      </c>
+      <c r="AE3" s="20">
+        <v>1.8391444178829401</v>
+      </c>
+      <c r="AF3" s="20">
+        <v>1.8747682617819925</v>
+      </c>
+      <c r="AG3" s="20">
+        <v>1.9037214287348594</v>
+      </c>
+      <c r="AH3" s="20">
+        <v>1.9330171998608836</v>
+      </c>
+      <c r="AI3" s="20">
+        <v>1.9626584009867136</v>
+      </c>
+      <c r="AJ3" s="20">
+        <v>1.9926478711876765</v>
+      </c>
+      <c r="AK3" s="20">
+        <v>2.0229884628030699</v>
+      </c>
+      <c r="AL3" s="20">
+        <v>2.0465590535637337</v>
+      </c>
+      <c r="AM3" s="20">
+        <v>2.0703402523753147</v>
+      </c>
+      <c r="AN3" s="20">
+        <v>2.0943333720806838</v>
+      </c>
+      <c r="AO3" s="20">
+        <v>2.1185397301785733</v>
+      </c>
+      <c r="AP3" s="20">
+        <v>2.1429606488276343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1.130436</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1.3405151997302078</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1.155981494838745</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1.3158819494067027</v>
+      </c>
+      <c r="N4" s="20">
+        <v>1.228027468725523</v>
+      </c>
+      <c r="O4" s="20">
+        <v>1.2225466516920374</v>
+      </c>
+      <c r="P4" s="20">
+        <v>1.2642991758160602</v>
+      </c>
+      <c r="Q4" s="20">
+        <v>1.3061603371669015</v>
+      </c>
+      <c r="R4" s="20">
+        <v>1.3457029459936605</v>
+      </c>
+      <c r="S4" s="20">
+        <v>1.385820995226948</v>
+      </c>
+      <c r="T4" s="20">
+        <v>1.4283570465266955</v>
+      </c>
+      <c r="U4" s="20">
+        <v>1.4693026793705557</v>
+      </c>
+      <c r="V4" s="20">
+        <v>1.5100626733919791</v>
+      </c>
+      <c r="W4" s="20">
+        <v>1.5470140015439409</v>
+      </c>
+      <c r="X4" s="20">
+        <v>1.5846567014175537</v>
+      </c>
+      <c r="Y4" s="20">
+        <v>1.6229997712220672</v>
+      </c>
+      <c r="Z4" s="20">
+        <v>1.6620522756006084</v>
+      </c>
+      <c r="AA4" s="20">
+        <v>1.70182334575065</v>
+      </c>
+      <c r="AB4" s="20">
+        <v>1.7353881862675751</v>
+      </c>
+      <c r="AC4" s="20">
+        <v>1.7694597550384985</v>
+      </c>
+      <c r="AD4" s="20">
+        <v>1.804043379247714</v>
+      </c>
+      <c r="AE4" s="20">
+        <v>1.8391444178829401</v>
+      </c>
+      <c r="AF4" s="20">
+        <v>1.8747682617819925</v>
+      </c>
+      <c r="AG4" s="20">
+        <v>1.9037214287348594</v>
+      </c>
+      <c r="AH4" s="20">
+        <v>1.9330171998608836</v>
+      </c>
+      <c r="AI4" s="20">
+        <v>1.9626584009867136</v>
+      </c>
+      <c r="AJ4" s="20">
+        <v>1.9926478711876765</v>
+      </c>
+      <c r="AK4" s="20">
+        <v>2.0229884628030699</v>
+      </c>
+      <c r="AL4" s="20">
+        <v>2.0465590535637337</v>
+      </c>
+      <c r="AM4" s="20">
+        <v>2.0703402523753147</v>
+      </c>
+      <c r="AN4" s="20">
+        <v>2.0943333720806838</v>
+      </c>
+      <c r="AO4" s="20">
+        <v>2.1185397301785733</v>
+      </c>
+      <c r="AP4" s="20">
+        <v>2.1429606488276343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1.130436</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1.3405151997302078</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1.155981494838745</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1.3158819494067027</v>
+      </c>
+      <c r="N5" s="20">
+        <v>1.228027468725523</v>
+      </c>
+      <c r="O5" s="20">
+        <v>1.2225466516920374</v>
+      </c>
+      <c r="P5" s="20">
+        <v>1.2642991758160602</v>
+      </c>
+      <c r="Q5" s="20">
+        <v>1.3061603371669015</v>
+      </c>
+      <c r="R5" s="20">
+        <v>1.3457029459936605</v>
+      </c>
+      <c r="S5" s="20">
+        <v>1.385820995226948</v>
+      </c>
+      <c r="T5" s="20">
+        <v>1.4283570465266955</v>
+      </c>
+      <c r="U5" s="20">
+        <v>1.4693026793705557</v>
+      </c>
+      <c r="V5" s="20">
+        <v>1.5100626733919791</v>
+      </c>
+      <c r="W5" s="20">
+        <v>1.5470140015439409</v>
+      </c>
+      <c r="X5" s="20">
+        <v>1.5846567014175537</v>
+      </c>
+      <c r="Y5" s="20">
+        <v>1.6229997712220672</v>
+      </c>
+      <c r="Z5" s="20">
+        <v>1.6620522756006084</v>
+      </c>
+      <c r="AA5" s="20">
+        <v>1.70182334575065</v>
+      </c>
+      <c r="AB5" s="20">
+        <v>1.7353881862675751</v>
+      </c>
+      <c r="AC5" s="20">
+        <v>1.7694597550384985</v>
+      </c>
+      <c r="AD5" s="20">
+        <v>1.804043379247714</v>
+      </c>
+      <c r="AE5" s="20">
+        <v>1.8391444178829401</v>
+      </c>
+      <c r="AF5" s="20">
+        <v>1.8747682617819925</v>
+      </c>
+      <c r="AG5" s="20">
+        <v>1.9037214287348594</v>
+      </c>
+      <c r="AH5" s="20">
+        <v>1.9330171998608836</v>
+      </c>
+      <c r="AI5" s="20">
+        <v>1.9626584009867136</v>
+      </c>
+      <c r="AJ5" s="20">
+        <v>1.9926478711876765</v>
+      </c>
+      <c r="AK5" s="20">
+        <v>2.0229884628030699</v>
+      </c>
+      <c r="AL5" s="20">
+        <v>2.0465590535637337</v>
+      </c>
+      <c r="AM5" s="20">
+        <v>2.0703402523753147</v>
+      </c>
+      <c r="AN5" s="20">
+        <v>2.0943333720806838</v>
+      </c>
+      <c r="AO5" s="20">
+        <v>2.1185397301785733</v>
+      </c>
+      <c r="AP5" s="20">
+        <v>2.1429606488276343</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" customWidth="1"/>
-    <col min="5" max="5" width="20.36328125" customWidth="1"/>
-    <col min="6" max="6" width="27.36328125" customWidth="1"/>
-    <col min="7" max="7" width="20.6328125" customWidth="1"/>
-    <col min="8" max="8" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="41" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="41" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2001,7 +2682,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2126,7 +2807,7 @@
         <v>2.1429606488276343</v>
       </c>
     </row>
-    <row r="3" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2251,7 +2932,7 @@
         <v>2.815711300630849E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2376,7 +3057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2501,7 +3182,7 @@
         <v>4.3419553449942834</v>
       </c>
     </row>
-    <row r="6" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2626,7 +3307,7 @@
         <v>31.783745522561652</v>
       </c>
     </row>
-    <row r="7" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2751,7 +3432,7 @@
         <v>4.679535458273743E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2876,7 +3557,7 @@
         <v>11.909343244170859</v>
       </c>
     </row>
-    <row r="9" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -3001,7 +3682,7 @@
         <v>0.15664824743805622</v>
       </c>
     </row>
-    <row r="10" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -3126,7 +3807,7 @@
         <v>7.059140590019382</v>
       </c>
     </row>
-    <row r="11" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -3251,7 +3932,7 @@
         <v>4.0686708613328726</v>
       </c>
     </row>
-    <row r="12" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -3376,7 +4057,7 @@
         <v>44.621612728492487</v>
       </c>
     </row>
-    <row r="13" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -3501,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -3626,7 +4307,7 @@
         <v>34.198284730741726</v>
       </c>
     </row>
-    <row r="15" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -3751,7 +4432,7 @@
         <v>15.809342976624043</v>
       </c>
     </row>
-    <row r="16" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -3876,7 +4557,7 @@
         <v>6.7148498166042838</v>
       </c>
     </row>
-    <row r="17" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -4001,7 +4682,7 @@
         <v>38.294453778208833</v>
       </c>
     </row>
-    <row r="18" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -4126,7 +4807,7 @@
         <v>39.772943840556849</v>
       </c>
     </row>
-    <row r="19" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -4251,7 +4932,7 @@
         <v>44.017558871941681</v>
       </c>
     </row>
-    <row r="20" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -4376,7 +5057,7 @@
         <v>0.9260819694806034</v>
       </c>
     </row>
-    <row r="21" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -4501,7 +5182,7 @@
         <v>38.018691037914365</v>
       </c>
     </row>
-    <row r="22" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4626,7 +5307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -4751,7 +5432,7 @@
         <v>3.534512538735572</v>
       </c>
     </row>
-    <row r="24" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -4876,7 +5557,7 @@
         <v>1.376490829749679</v>
       </c>
     </row>
-    <row r="25" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -5001,7 +5682,7 @@
         <v>2.8789249787271318</v>
       </c>
     </row>
-    <row r="26" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
@@ -5126,7 +5807,7 @@
         <v>41.893231854046718</v>
       </c>
     </row>
-    <row r="27" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -5251,7 +5932,7 @@
         <v>0.22562613925805353</v>
       </c>
     </row>
-    <row r="28" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -5376,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -5501,7 +6182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -5626,7 +6307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -5751,7 +6432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5876,7 +6557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -6001,7 +6682,7 @@
         <v>5.8116811685614573</v>
       </c>
     </row>
-    <row r="34" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -6126,7 +6807,7 @@
         <v>8.8815348710376121</v>
       </c>
     </row>
-    <row r="35" spans="1:41" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:41" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -6251,7 +6932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
         <v>8</v>
       </c>
@@ -6376,7 +7057,7 @@
         <v>0.73968433888862206</v>
       </c>
     </row>
-    <row r="37" spans="1:41" s="3" customFormat="1" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:41" s="3" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
         <v>8</v>
       </c>
@@ -6501,7 +7182,7 @@
         <v>0.9041109388705898</v>
       </c>
     </row>
-    <row r="38" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="30" t="s">
         <v>8</v>
       </c>
@@ -6626,7 +7307,7 @@
         <v>3.237330536821851</v>
       </c>
     </row>
-    <row r="39" spans="1:41" s="3" customFormat="1" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:41" s="3" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="30" t="s">
         <v>8</v>
       </c>
@@ -6751,7 +7432,7 @@
         <v>3.6936017993242053E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="30" t="s">
         <v>8</v>
       </c>
@@ -6876,7 +7557,7 @@
         <v>0.10891297933424089</v>
       </c>
     </row>
-    <row r="41" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="30" t="s">
         <v>8</v>
       </c>
@@ -7001,7 +7682,7 @@
         <v>0.55828955953503578</v>
       </c>
     </row>
-    <row r="42" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="30" t="s">
         <v>8</v>
       </c>
@@ -7126,7 +7807,7 @@
         <v>0.53562056641812317</v>
       </c>
     </row>
-    <row r="43" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="30" t="s">
         <v>8</v>
       </c>
@@ -7251,7 +7932,7 @@
         <v>0.3308293136222733</v>
       </c>
     </row>
-    <row r="44" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="30" t="s">
         <v>8</v>
       </c>
@@ -7376,7 +8057,7 @@
         <v>2.3563643081164449</v>
       </c>
     </row>
-    <row r="45" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="30" t="s">
         <v>8</v>
       </c>
@@ -7501,7 +8182,7 @@
         <v>0.3096676051461088</v>
       </c>
     </row>
-    <row r="46" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="30" t="s">
         <v>8</v>
       </c>
@@ -7626,7 +8307,7 @@
         <v>2.8044446154538938</v>
       </c>
     </row>
-    <row r="47" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="30" t="s">
         <v>8</v>
       </c>
@@ -7751,7 +8432,7 @@
         <v>0.48962516783660348</v>
       </c>
     </row>
-    <row r="48" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="30" t="s">
         <v>8</v>
       </c>
@@ -7876,7 +8557,7 @@
         <v>5.7639777025201941E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="30" t="s">
         <v>8</v>
       </c>
@@ -8001,7 +8682,7 @@
         <v>3.8619398403142949E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="30" t="s">
         <v>8</v>
       </c>
@@ -8126,7 +8807,7 @@
         <v>6.5551550140085998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="30" t="s">
         <v>8</v>
       </c>
@@ -8251,7 +8932,7 @@
         <v>5.425717717790729E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="68" t="s">
         <v>8</v>
       </c>
@@ -8376,7 +9057,7 @@
         <v>3.5824311010091768E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="75" t="s">
         <v>8</v>
       </c>
@@ -8501,7 +9182,7 @@
         <v>4.4290205807614662E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="79" t="s">
         <v>8</v>
       </c>
@@ -8626,7 +9307,7 @@
         <v>6.3423574716504186E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="81" t="s">
         <v>8</v>
       </c>
@@ -8751,7 +9432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="79" t="s">
         <v>8</v>
       </c>
@@ -8876,7 +9557,7 @@
         <v>0.13075886040993689</v>
       </c>
     </row>
-    <row r="57" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="79" t="s">
         <v>8</v>
       </c>
@@ -9001,7 +9682,7 @@
         <v>3.543216464609172E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="79" t="s">
         <v>8</v>
       </c>
@@ -9126,7 +9807,7 @@
         <v>1.771608232304586E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="79" t="s">
         <v>8</v>
       </c>
@@ -9251,7 +9932,7 @@
         <v>7.8143867518722987E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="79" t="s">
         <v>8</v>
       </c>
@@ -9376,7 +10057,7 @@
         <v>0.87930585715619991</v>
       </c>
     </row>
-    <row r="61" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="79" t="s">
         <v>8</v>
       </c>
@@ -9501,7 +10182,7 @@
         <v>2.4044072051932282E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="79" t="s">
         <v>8</v>
       </c>
@@ -9626,7 +10307,7 @@
         <v>0.1559015244428035</v>
       </c>
     </row>
-    <row r="63" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="79" t="s">
         <v>8</v>
       </c>
@@ -9751,7 +10432,7 @@
         <v>0.51376638736832991</v>
       </c>
     </row>
-    <row r="64" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="79" t="s">
         <v>8</v>
       </c>
@@ -9876,7 +10557,7 @@
         <v>1.792760992344606E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="79" t="s">
         <v>8</v>
       </c>
@@ -10001,7 +10682,7 @@
         <v>6.418084352593692E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="79" t="s">
         <v>8</v>
       </c>
@@ -10126,7 +10807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="79" t="s">
         <v>8</v>
       </c>
@@ -10251,7 +10932,7 @@
         <v>0.13232010332297073</v>
       </c>
     </row>
-    <row r="68" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="79" t="s">
         <v>8</v>
       </c>
@@ -10376,7 +11057,7 @@
         <v>0.12549326946412248</v>
       </c>
     </row>
-    <row r="69" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="86" t="s">
         <v>8</v>
       </c>
@@ -10501,7 +11182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>8</v>
       </c>
@@ -10626,7 +11307,7 @@
         <v>7.6296369378360556</v>
       </c>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>8</v>
       </c>
@@ -10751,7 +11432,7 @@
         <v>2.2652999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
         <v>8</v>
       </c>
@@ -10876,7 +11557,7 @@
         <v>12.277200000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A73" s="39" t="s">
         <v>8</v>
       </c>
@@ -10905,7 +11586,7 @@
         <v>59.785899999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A74" s="39" t="s">
         <v>124</v>
       </c>
@@ -10934,7 +11615,7 @@
         <v>0.38750000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A75" s="39" t="s">
         <v>124</v>
       </c>
@@ -10963,7 +11644,7 @@
         <v>0.38750000000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A76" s="39" t="s">
         <v>124</v>
       </c>
@@ -10992,7 +11673,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
         <v>8</v>
       </c>
@@ -11021,7 +11702,7 @@
         <v>28.942299999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A78" s="39" t="s">
         <v>124</v>
       </c>
@@ -11050,7 +11731,7 @@
         <v>6.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A79" s="39" t="s">
         <v>124</v>
       </c>
@@ -11079,7 +11760,7 @@
         <v>0.33529999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A80" s="39" t="s">
         <v>124</v>
       </c>
@@ -11108,7 +11789,7 @@
         <v>0.65800000000000003</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="39" t="s">
         <v>124</v>
       </c>
@@ -11137,7 +11818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="39" t="s">
         <v>124</v>
       </c>
@@ -11166,7 +11847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="39" t="s">
         <v>8</v>
       </c>
@@ -11195,7 +11876,7 @@
         <v>14.555999999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="39" t="s">
         <v>124</v>
       </c>
@@ -11224,7 +11905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="39" t="s">
         <v>8</v>
       </c>
@@ -11253,7 +11934,7 @@
         <v>12.510999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="39" t="s">
         <v>124</v>
       </c>
@@ -11282,7 +11963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="39" t="s">
         <v>124</v>
       </c>
@@ -11311,7 +11992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="39" t="s">
         <v>8</v>
       </c>
@@ -11340,7 +12021,7 @@
         <v>15.461</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="39" t="s">
         <v>124</v>
       </c>
@@ -11369,7 +12050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="39" t="s">
         <v>8</v>
       </c>
@@ -11407,6 +12088,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -11415,7 +12106,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -11646,29 +12337,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ED672C9-E834-4E4B-BB43-E87E9628BAF2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{124352EC-5983-47FF-B2F1-21582D939B66}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EFBB33F-3B30-4D18-BAAC-D5F71240E8ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11677,4 +12346,31 @@
     <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ED672C9-E834-4E4B-BB43-E87E9628BAF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{124352EC-5983-47FF-B2F1-21582D939B66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correct the Timeslices use for the example
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Outputs/A-O_Demand.xlsx
+++ b/t1_confection/A1_Outputs/A-O_Demand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t1_confection\A1_Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0DABE5-3865-424E-B0CA-4F2027C862BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752F78AE-F444-40B3-AFEF-49DF7BD35389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5370" yWindow="2490" windowWidth="21630" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeslices" sheetId="3" r:id="rId1"/>
@@ -855,10 +855,10 @@
     <t>Timeslice</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>P2</t>
+    <t>DRY</t>
+  </si>
+  <si>
+    <t>RAIN</t>
   </si>
 </sst>
 </file>
@@ -1870,7 +1870,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD5"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12088,25 +12088,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -12337,26 +12318,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EFBB33F-3B30-4D18-BAAC-D5F71240E8ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
-    <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ED672C9-E834-4E4B-BB43-E87E9628BAF2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{124352EC-5983-47FF-B2F1-21582D939B66}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12373,4 +12354,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ED672C9-E834-4E4B-BB43-E87E9628BAF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EFBB33F-3B30-4D18-BAAC-D5F71240E8ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correct condiction for concatenate script and Demand and Parametrization excels about timeslices
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Outputs/A-O_Demand.xlsx
+++ b/t1_confection/A1_Outputs/A-O_Demand.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisfernando\Dropbox\2_WORK\MOMF\RD_Model_v9_clean_new\A1_Outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t1_confection\A1_Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303696FF-3226-44B4-B338-F5CC94F5BAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752F78AE-F444-40B3-AFEF-49DF7BD35389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5370" yWindow="2490" windowWidth="21630" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Demand_Projection" sheetId="1" r:id="rId1"/>
+    <sheet name="Timeslices" sheetId="3" r:id="rId1"/>
+    <sheet name="Demand_Projection" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -351,7 +352,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="169">
   <si>
     <t>Demand/Share</t>
   </si>
@@ -849,6 +850,15 @@
   </si>
   <si>
     <t>Transport Demand non motorized reductions</t>
+  </si>
+  <si>
+    <t>Timeslice</t>
+  </si>
+  <si>
+    <t>DRY</t>
+  </si>
+  <si>
+    <t>RAIN</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1530,6 +1540,7 @@
     <xf numFmtId="166" fontId="6" fillId="13" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1854,29 +1865,699 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037C0E4B-223C-493A-AA95-0D314598A9DF}">
+  <dimension ref="A1:AP5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A1" s="91" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2023</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2024</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2026</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2027</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2028</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2029</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2030</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2031</v>
+      </c>
+      <c r="X1" s="1">
+        <v>2032</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>2033</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>2034</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>2035</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>2036</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>2037</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>2038</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>2039</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>2040</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>2041</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>2042</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>2043</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>2044</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>2045</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>2046</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>2047</v>
+      </c>
+      <c r="AN1" s="1">
+        <v>2048</v>
+      </c>
+      <c r="AO1" s="1">
+        <v>2049</v>
+      </c>
+      <c r="AP1" s="1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1.130436</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1.3405151997302078</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1.155981494838745</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1.3158819494067027</v>
+      </c>
+      <c r="N2" s="20">
+        <v>1.228027468725523</v>
+      </c>
+      <c r="O2" s="20">
+        <v>1.2225466516920374</v>
+      </c>
+      <c r="P2" s="20">
+        <v>1.2642991758160602</v>
+      </c>
+      <c r="Q2" s="20">
+        <v>1.3061603371669015</v>
+      </c>
+      <c r="R2" s="20">
+        <v>1.3457029459936605</v>
+      </c>
+      <c r="S2" s="20">
+        <v>1.385820995226948</v>
+      </c>
+      <c r="T2" s="20">
+        <v>1.4283570465266955</v>
+      </c>
+      <c r="U2" s="20">
+        <v>1.4693026793705557</v>
+      </c>
+      <c r="V2" s="20">
+        <v>1.5100626733919791</v>
+      </c>
+      <c r="W2" s="20">
+        <v>1.5470140015439409</v>
+      </c>
+      <c r="X2" s="20">
+        <v>1.5846567014175537</v>
+      </c>
+      <c r="Y2" s="20">
+        <v>1.6229997712220672</v>
+      </c>
+      <c r="Z2" s="20">
+        <v>1.6620522756006084</v>
+      </c>
+      <c r="AA2" s="20">
+        <v>1.70182334575065</v>
+      </c>
+      <c r="AB2" s="20">
+        <v>1.7353881862675751</v>
+      </c>
+      <c r="AC2" s="20">
+        <v>1.7694597550384985</v>
+      </c>
+      <c r="AD2" s="20">
+        <v>1.804043379247714</v>
+      </c>
+      <c r="AE2" s="20">
+        <v>1.8391444178829401</v>
+      </c>
+      <c r="AF2" s="20">
+        <v>1.8747682617819925</v>
+      </c>
+      <c r="AG2" s="20">
+        <v>1.9037214287348594</v>
+      </c>
+      <c r="AH2" s="20">
+        <v>1.9330171998608836</v>
+      </c>
+      <c r="AI2" s="20">
+        <v>1.9626584009867136</v>
+      </c>
+      <c r="AJ2" s="20">
+        <v>1.9926478711876765</v>
+      </c>
+      <c r="AK2" s="20">
+        <v>2.0229884628030699</v>
+      </c>
+      <c r="AL2" s="20">
+        <v>2.0465590535637337</v>
+      </c>
+      <c r="AM2" s="20">
+        <v>2.0703402523753147</v>
+      </c>
+      <c r="AN2" s="20">
+        <v>2.0943333720806838</v>
+      </c>
+      <c r="AO2" s="20">
+        <v>2.1185397301785733</v>
+      </c>
+      <c r="AP2" s="20">
+        <v>2.1429606488276343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.130436</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1.3405151997302078</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1.155981494838745</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1.3158819494067027</v>
+      </c>
+      <c r="N3" s="20">
+        <v>1.228027468725523</v>
+      </c>
+      <c r="O3" s="20">
+        <v>1.2225466516920374</v>
+      </c>
+      <c r="P3" s="20">
+        <v>1.2642991758160602</v>
+      </c>
+      <c r="Q3" s="20">
+        <v>1.3061603371669015</v>
+      </c>
+      <c r="R3" s="20">
+        <v>1.3457029459936605</v>
+      </c>
+      <c r="S3" s="20">
+        <v>1.385820995226948</v>
+      </c>
+      <c r="T3" s="20">
+        <v>1.4283570465266955</v>
+      </c>
+      <c r="U3" s="20">
+        <v>1.4693026793705557</v>
+      </c>
+      <c r="V3" s="20">
+        <v>1.5100626733919791</v>
+      </c>
+      <c r="W3" s="20">
+        <v>1.5470140015439409</v>
+      </c>
+      <c r="X3" s="20">
+        <v>1.5846567014175537</v>
+      </c>
+      <c r="Y3" s="20">
+        <v>1.6229997712220672</v>
+      </c>
+      <c r="Z3" s="20">
+        <v>1.6620522756006084</v>
+      </c>
+      <c r="AA3" s="20">
+        <v>1.70182334575065</v>
+      </c>
+      <c r="AB3" s="20">
+        <v>1.7353881862675751</v>
+      </c>
+      <c r="AC3" s="20">
+        <v>1.7694597550384985</v>
+      </c>
+      <c r="AD3" s="20">
+        <v>1.804043379247714</v>
+      </c>
+      <c r="AE3" s="20">
+        <v>1.8391444178829401</v>
+      </c>
+      <c r="AF3" s="20">
+        <v>1.8747682617819925</v>
+      </c>
+      <c r="AG3" s="20">
+        <v>1.9037214287348594</v>
+      </c>
+      <c r="AH3" s="20">
+        <v>1.9330171998608836</v>
+      </c>
+      <c r="AI3" s="20">
+        <v>1.9626584009867136</v>
+      </c>
+      <c r="AJ3" s="20">
+        <v>1.9926478711876765</v>
+      </c>
+      <c r="AK3" s="20">
+        <v>2.0229884628030699</v>
+      </c>
+      <c r="AL3" s="20">
+        <v>2.0465590535637337</v>
+      </c>
+      <c r="AM3" s="20">
+        <v>2.0703402523753147</v>
+      </c>
+      <c r="AN3" s="20">
+        <v>2.0943333720806838</v>
+      </c>
+      <c r="AO3" s="20">
+        <v>2.1185397301785733</v>
+      </c>
+      <c r="AP3" s="20">
+        <v>2.1429606488276343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1.130436</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1.3405151997302078</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1.155981494838745</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1.3158819494067027</v>
+      </c>
+      <c r="N4" s="20">
+        <v>1.228027468725523</v>
+      </c>
+      <c r="O4" s="20">
+        <v>1.2225466516920374</v>
+      </c>
+      <c r="P4" s="20">
+        <v>1.2642991758160602</v>
+      </c>
+      <c r="Q4" s="20">
+        <v>1.3061603371669015</v>
+      </c>
+      <c r="R4" s="20">
+        <v>1.3457029459936605</v>
+      </c>
+      <c r="S4" s="20">
+        <v>1.385820995226948</v>
+      </c>
+      <c r="T4" s="20">
+        <v>1.4283570465266955</v>
+      </c>
+      <c r="U4" s="20">
+        <v>1.4693026793705557</v>
+      </c>
+      <c r="V4" s="20">
+        <v>1.5100626733919791</v>
+      </c>
+      <c r="W4" s="20">
+        <v>1.5470140015439409</v>
+      </c>
+      <c r="X4" s="20">
+        <v>1.5846567014175537</v>
+      </c>
+      <c r="Y4" s="20">
+        <v>1.6229997712220672</v>
+      </c>
+      <c r="Z4" s="20">
+        <v>1.6620522756006084</v>
+      </c>
+      <c r="AA4" s="20">
+        <v>1.70182334575065</v>
+      </c>
+      <c r="AB4" s="20">
+        <v>1.7353881862675751</v>
+      </c>
+      <c r="AC4" s="20">
+        <v>1.7694597550384985</v>
+      </c>
+      <c r="AD4" s="20">
+        <v>1.804043379247714</v>
+      </c>
+      <c r="AE4" s="20">
+        <v>1.8391444178829401</v>
+      </c>
+      <c r="AF4" s="20">
+        <v>1.8747682617819925</v>
+      </c>
+      <c r="AG4" s="20">
+        <v>1.9037214287348594</v>
+      </c>
+      <c r="AH4" s="20">
+        <v>1.9330171998608836</v>
+      </c>
+      <c r="AI4" s="20">
+        <v>1.9626584009867136</v>
+      </c>
+      <c r="AJ4" s="20">
+        <v>1.9926478711876765</v>
+      </c>
+      <c r="AK4" s="20">
+        <v>2.0229884628030699</v>
+      </c>
+      <c r="AL4" s="20">
+        <v>2.0465590535637337</v>
+      </c>
+      <c r="AM4" s="20">
+        <v>2.0703402523753147</v>
+      </c>
+      <c r="AN4" s="20">
+        <v>2.0943333720806838</v>
+      </c>
+      <c r="AO4" s="20">
+        <v>2.1185397301785733</v>
+      </c>
+      <c r="AP4" s="20">
+        <v>2.1429606488276343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1.130436</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1.3405151997302078</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1.155981494838745</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1.3158819494067027</v>
+      </c>
+      <c r="N5" s="20">
+        <v>1.228027468725523</v>
+      </c>
+      <c r="O5" s="20">
+        <v>1.2225466516920374</v>
+      </c>
+      <c r="P5" s="20">
+        <v>1.2642991758160602</v>
+      </c>
+      <c r="Q5" s="20">
+        <v>1.3061603371669015</v>
+      </c>
+      <c r="R5" s="20">
+        <v>1.3457029459936605</v>
+      </c>
+      <c r="S5" s="20">
+        <v>1.385820995226948</v>
+      </c>
+      <c r="T5" s="20">
+        <v>1.4283570465266955</v>
+      </c>
+      <c r="U5" s="20">
+        <v>1.4693026793705557</v>
+      </c>
+      <c r="V5" s="20">
+        <v>1.5100626733919791</v>
+      </c>
+      <c r="W5" s="20">
+        <v>1.5470140015439409</v>
+      </c>
+      <c r="X5" s="20">
+        <v>1.5846567014175537</v>
+      </c>
+      <c r="Y5" s="20">
+        <v>1.6229997712220672</v>
+      </c>
+      <c r="Z5" s="20">
+        <v>1.6620522756006084</v>
+      </c>
+      <c r="AA5" s="20">
+        <v>1.70182334575065</v>
+      </c>
+      <c r="AB5" s="20">
+        <v>1.7353881862675751</v>
+      </c>
+      <c r="AC5" s="20">
+        <v>1.7694597550384985</v>
+      </c>
+      <c r="AD5" s="20">
+        <v>1.804043379247714</v>
+      </c>
+      <c r="AE5" s="20">
+        <v>1.8391444178829401</v>
+      </c>
+      <c r="AF5" s="20">
+        <v>1.8747682617819925</v>
+      </c>
+      <c r="AG5" s="20">
+        <v>1.9037214287348594</v>
+      </c>
+      <c r="AH5" s="20">
+        <v>1.9330171998608836</v>
+      </c>
+      <c r="AI5" s="20">
+        <v>1.9626584009867136</v>
+      </c>
+      <c r="AJ5" s="20">
+        <v>1.9926478711876765</v>
+      </c>
+      <c r="AK5" s="20">
+        <v>2.0229884628030699</v>
+      </c>
+      <c r="AL5" s="20">
+        <v>2.0465590535637337</v>
+      </c>
+      <c r="AM5" s="20">
+        <v>2.0703402523753147</v>
+      </c>
+      <c r="AN5" s="20">
+        <v>2.0943333720806838</v>
+      </c>
+      <c r="AO5" s="20">
+        <v>2.1185397301785733</v>
+      </c>
+      <c r="AP5" s="20">
+        <v>2.1429606488276343</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" customWidth="1"/>
-    <col min="5" max="5" width="20.36328125" customWidth="1"/>
-    <col min="6" max="6" width="27.36328125" customWidth="1"/>
-    <col min="7" max="7" width="20.6328125" customWidth="1"/>
-    <col min="8" max="8" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="41" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="41" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2001,7 +2682,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2126,7 +2807,7 @@
         <v>2.1429606488276343</v>
       </c>
     </row>
-    <row r="3" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2251,7 +2932,7 @@
         <v>2.815711300630849E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2376,7 +3057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2501,7 +3182,7 @@
         <v>4.3419553449942834</v>
       </c>
     </row>
-    <row r="6" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2626,7 +3307,7 @@
         <v>31.783745522561652</v>
       </c>
     </row>
-    <row r="7" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2751,7 +3432,7 @@
         <v>4.679535458273743E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2876,7 +3557,7 @@
         <v>11.909343244170859</v>
       </c>
     </row>
-    <row r="9" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -3001,7 +3682,7 @@
         <v>0.15664824743805622</v>
       </c>
     </row>
-    <row r="10" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -3126,7 +3807,7 @@
         <v>7.059140590019382</v>
       </c>
     </row>
-    <row r="11" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -3251,7 +3932,7 @@
         <v>4.0686708613328726</v>
       </c>
     </row>
-    <row r="12" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -3376,7 +4057,7 @@
         <v>44.621612728492487</v>
       </c>
     </row>
-    <row r="13" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -3501,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -3626,7 +4307,7 @@
         <v>34.198284730741726</v>
       </c>
     </row>
-    <row r="15" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -3751,7 +4432,7 @@
         <v>15.809342976624043</v>
       </c>
     </row>
-    <row r="16" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -3876,7 +4557,7 @@
         <v>6.7148498166042838</v>
       </c>
     </row>
-    <row r="17" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -4001,7 +4682,7 @@
         <v>38.294453778208833</v>
       </c>
     </row>
-    <row r="18" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -4126,7 +4807,7 @@
         <v>39.772943840556849</v>
       </c>
     </row>
-    <row r="19" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -4251,7 +4932,7 @@
         <v>44.017558871941681</v>
       </c>
     </row>
-    <row r="20" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -4376,7 +5057,7 @@
         <v>0.9260819694806034</v>
       </c>
     </row>
-    <row r="21" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -4501,7 +5182,7 @@
         <v>38.018691037914365</v>
       </c>
     </row>
-    <row r="22" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4626,7 +5307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -4751,7 +5432,7 @@
         <v>3.534512538735572</v>
       </c>
     </row>
-    <row r="24" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -4876,7 +5557,7 @@
         <v>1.376490829749679</v>
       </c>
     </row>
-    <row r="25" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -5001,7 +5682,7 @@
         <v>2.8789249787271318</v>
       </c>
     </row>
-    <row r="26" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
@@ -5126,7 +5807,7 @@
         <v>41.893231854046718</v>
       </c>
     </row>
-    <row r="27" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -5251,7 +5932,7 @@
         <v>0.22562613925805353</v>
       </c>
     </row>
-    <row r="28" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -5376,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -5501,7 +6182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -5626,7 +6307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -5751,7 +6432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5876,7 +6557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -6001,7 +6682,7 @@
         <v>5.8116811685614573</v>
       </c>
     </row>
-    <row r="34" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -6126,7 +6807,7 @@
         <v>8.8815348710376121</v>
       </c>
     </row>
-    <row r="35" spans="1:41" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:41" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -6251,7 +6932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
         <v>8</v>
       </c>
@@ -6376,7 +7057,7 @@
         <v>0.73968433888862206</v>
       </c>
     </row>
-    <row r="37" spans="1:41" s="3" customFormat="1" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:41" s="3" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
         <v>8</v>
       </c>
@@ -6501,7 +7182,7 @@
         <v>0.9041109388705898</v>
       </c>
     </row>
-    <row r="38" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="30" t="s">
         <v>8</v>
       </c>
@@ -6626,7 +7307,7 @@
         <v>3.237330536821851</v>
       </c>
     </row>
-    <row r="39" spans="1:41" s="3" customFormat="1" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:41" s="3" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="30" t="s">
         <v>8</v>
       </c>
@@ -6751,7 +7432,7 @@
         <v>3.6936017993242053E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="30" t="s">
         <v>8</v>
       </c>
@@ -6876,7 +7557,7 @@
         <v>0.10891297933424089</v>
       </c>
     </row>
-    <row r="41" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="30" t="s">
         <v>8</v>
       </c>
@@ -7001,7 +7682,7 @@
         <v>0.55828955953503578</v>
       </c>
     </row>
-    <row r="42" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="30" t="s">
         <v>8</v>
       </c>
@@ -7126,7 +7807,7 @@
         <v>0.53562056641812317</v>
       </c>
     </row>
-    <row r="43" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="30" t="s">
         <v>8</v>
       </c>
@@ -7251,7 +7932,7 @@
         <v>0.3308293136222733</v>
       </c>
     </row>
-    <row r="44" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="30" t="s">
         <v>8</v>
       </c>
@@ -7376,7 +8057,7 @@
         <v>2.3563643081164449</v>
       </c>
     </row>
-    <row r="45" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="30" t="s">
         <v>8</v>
       </c>
@@ -7501,7 +8182,7 @@
         <v>0.3096676051461088</v>
       </c>
     </row>
-    <row r="46" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="30" t="s">
         <v>8</v>
       </c>
@@ -7626,7 +8307,7 @@
         <v>2.8044446154538938</v>
       </c>
     </row>
-    <row r="47" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="30" t="s">
         <v>8</v>
       </c>
@@ -7751,7 +8432,7 @@
         <v>0.48962516783660348</v>
       </c>
     </row>
-    <row r="48" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="30" t="s">
         <v>8</v>
       </c>
@@ -7876,7 +8557,7 @@
         <v>5.7639777025201941E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="30" t="s">
         <v>8</v>
       </c>
@@ -8001,7 +8682,7 @@
         <v>3.8619398403142949E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="30" t="s">
         <v>8</v>
       </c>
@@ -8126,7 +8807,7 @@
         <v>6.5551550140085998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="30" t="s">
         <v>8</v>
       </c>
@@ -8251,7 +8932,7 @@
         <v>5.425717717790729E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="68" t="s">
         <v>8</v>
       </c>
@@ -8376,7 +9057,7 @@
         <v>3.5824311010091768E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="75" t="s">
         <v>8</v>
       </c>
@@ -8501,7 +9182,7 @@
         <v>4.4290205807614662E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="79" t="s">
         <v>8</v>
       </c>
@@ -8626,7 +9307,7 @@
         <v>6.3423574716504186E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="81" t="s">
         <v>8</v>
       </c>
@@ -8751,7 +9432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="79" t="s">
         <v>8</v>
       </c>
@@ -8876,7 +9557,7 @@
         <v>0.13075886040993689</v>
       </c>
     </row>
-    <row r="57" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="79" t="s">
         <v>8</v>
       </c>
@@ -9001,7 +9682,7 @@
         <v>3.543216464609172E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="79" t="s">
         <v>8</v>
       </c>
@@ -9126,7 +9807,7 @@
         <v>1.771608232304586E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="79" t="s">
         <v>8</v>
       </c>
@@ -9251,7 +9932,7 @@
         <v>7.8143867518722987E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="79" t="s">
         <v>8</v>
       </c>
@@ -9376,7 +10057,7 @@
         <v>0.87930585715619991</v>
       </c>
     </row>
-    <row r="61" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="79" t="s">
         <v>8</v>
       </c>
@@ -9501,7 +10182,7 @@
         <v>2.4044072051932282E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="79" t="s">
         <v>8</v>
       </c>
@@ -9626,7 +10307,7 @@
         <v>0.1559015244428035</v>
       </c>
     </row>
-    <row r="63" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="79" t="s">
         <v>8</v>
       </c>
@@ -9751,7 +10432,7 @@
         <v>0.51376638736832991</v>
       </c>
     </row>
-    <row r="64" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="79" t="s">
         <v>8</v>
       </c>
@@ -9876,7 +10557,7 @@
         <v>1.792760992344606E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="79" t="s">
         <v>8</v>
       </c>
@@ -10001,7 +10682,7 @@
         <v>6.418084352593692E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="79" t="s">
         <v>8</v>
       </c>
@@ -10126,7 +10807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="79" t="s">
         <v>8</v>
       </c>
@@ -10251,7 +10932,7 @@
         <v>0.13232010332297073</v>
       </c>
     </row>
-    <row r="68" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="79" t="s">
         <v>8</v>
       </c>
@@ -10376,7 +11057,7 @@
         <v>0.12549326946412248</v>
       </c>
     </row>
-    <row r="69" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="86" t="s">
         <v>8</v>
       </c>
@@ -10501,7 +11182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>8</v>
       </c>
@@ -10626,7 +11307,7 @@
         <v>7.6296369378360556</v>
       </c>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>8</v>
       </c>
@@ -10751,7 +11432,7 @@
         <v>2.2652999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
         <v>8</v>
       </c>
@@ -10876,7 +11557,7 @@
         <v>12.277200000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A73" s="39" t="s">
         <v>8</v>
       </c>
@@ -10905,7 +11586,7 @@
         <v>59.785899999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A74" s="39" t="s">
         <v>124</v>
       </c>
@@ -10934,7 +11615,7 @@
         <v>0.38750000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A75" s="39" t="s">
         <v>124</v>
       </c>
@@ -10963,7 +11644,7 @@
         <v>0.38750000000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A76" s="39" t="s">
         <v>124</v>
       </c>
@@ -10992,7 +11673,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
         <v>8</v>
       </c>
@@ -11021,7 +11702,7 @@
         <v>28.942299999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A78" s="39" t="s">
         <v>124</v>
       </c>
@@ -11050,7 +11731,7 @@
         <v>6.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A79" s="39" t="s">
         <v>124</v>
       </c>
@@ -11079,7 +11760,7 @@
         <v>0.33529999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A80" s="39" t="s">
         <v>124</v>
       </c>
@@ -11108,7 +11789,7 @@
         <v>0.65800000000000003</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="39" t="s">
         <v>124</v>
       </c>
@@ -11137,7 +11818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="39" t="s">
         <v>124</v>
       </c>
@@ -11166,7 +11847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="39" t="s">
         <v>8</v>
       </c>
@@ -11195,7 +11876,7 @@
         <v>14.555999999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="39" t="s">
         <v>124</v>
       </c>
@@ -11224,7 +11905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="39" t="s">
         <v>8</v>
       </c>
@@ -11253,7 +11934,7 @@
         <v>12.510999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="39" t="s">
         <v>124</v>
       </c>
@@ -11282,7 +11963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="39" t="s">
         <v>124</v>
       </c>
@@ -11311,7 +11992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="39" t="s">
         <v>8</v>
       </c>
@@ -11340,7 +12021,7 @@
         <v>15.461</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="39" t="s">
         <v>124</v>
       </c>
@@ -11369,7 +12050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="39" t="s">
         <v>8</v>
       </c>
@@ -11407,15 +12088,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -11646,6 +12318,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11657,15 +12338,30 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{124352EC-5983-47FF-B2F1-21582D939B66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ED672C9-E834-4E4B-BB43-E87E9628BAF2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{124352EC-5983-47FF-B2F1-21582D939B66}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Correct condiction for concatenate script and in Uncertainty Table X_CAT=Average Distance .Also, Demand and Parametrization excels about timeslices
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Outputs/A-O_Demand.xlsx
+++ b/t1_confection/A1_Outputs/A-O_Demand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisfernando\Dropbox\2_WORK\MOMF\RD_Model_v9_clean_new\A1_Outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t1_confection\A1_Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303696FF-3226-44B4-B338-F5CC94F5BAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DBB3846-A01B-42D5-99CA-B33FA8066E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demand_Projection" sheetId="1" r:id="rId1"/>
@@ -1858,25 +1858,25 @@
   <dimension ref="A1:AO90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" customWidth="1"/>
-    <col min="5" max="5" width="20.36328125" customWidth="1"/>
-    <col min="6" max="6" width="27.36328125" customWidth="1"/>
-    <col min="7" max="7" width="20.6328125" customWidth="1"/>
-    <col min="8" max="8" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="41" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="41" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>2.1429606488276343</v>
       </c>
     </row>
-    <row r="3" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>2.815711300630849E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>4.3419553449942834</v>
       </c>
     </row>
-    <row r="6" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>31.783745522561652</v>
       </c>
     </row>
-    <row r="7" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>4.679535458273743E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>11.909343244170859</v>
       </c>
     </row>
-    <row r="9" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>0.15664824743805622</v>
       </c>
     </row>
-    <row r="10" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>7.059140590019382</v>
       </c>
     </row>
-    <row r="11" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>4.0686708613328726</v>
       </c>
     </row>
-    <row r="12" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>44.621612728492487</v>
       </c>
     </row>
-    <row r="13" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>34.198284730741726</v>
       </c>
     </row>
-    <row r="15" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>15.809342976624043</v>
       </c>
     </row>
-    <row r="16" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>6.7148498166042838</v>
       </c>
     </row>
-    <row r="17" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>38.294453778208833</v>
       </c>
     </row>
-    <row r="18" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>39.772943840556849</v>
       </c>
     </row>
-    <row r="19" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>44.017558871941681</v>
       </c>
     </row>
-    <row r="20" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -4376,7 +4376,7 @@
         <v>0.9260819694806034</v>
       </c>
     </row>
-    <row r="21" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>38.018691037914365</v>
       </c>
     </row>
-    <row r="22" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>3.534512538735572</v>
       </c>
     </row>
-    <row r="24" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -4876,7 +4876,7 @@
         <v>1.376490829749679</v>
       </c>
     </row>
-    <row r="25" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>2.8789249787271318</v>
       </c>
     </row>
-    <row r="26" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>41.893231854046718</v>
       </c>
     </row>
-    <row r="27" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>0.22562613925805353</v>
       </c>
     </row>
-    <row r="28" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -5376,7 +5376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -5876,7 +5876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>5.8116811685614573</v>
       </c>
     </row>
-    <row r="34" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -6126,7 +6126,7 @@
         <v>8.8815348710376121</v>
       </c>
     </row>
-    <row r="35" spans="1:41" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:41" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -6251,7 +6251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
         <v>8</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>0.73968433888862206</v>
       </c>
     </row>
-    <row r="37" spans="1:41" s="3" customFormat="1" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:41" s="3" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
         <v>8</v>
       </c>
@@ -6501,7 +6501,7 @@
         <v>0.9041109388705898</v>
       </c>
     </row>
-    <row r="38" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="30" t="s">
         <v>8</v>
       </c>
@@ -6626,7 +6626,7 @@
         <v>3.237330536821851</v>
       </c>
     </row>
-    <row r="39" spans="1:41" s="3" customFormat="1" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:41" s="3" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="30" t="s">
         <v>8</v>
       </c>
@@ -6751,7 +6751,7 @@
         <v>3.6936017993242053E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="30" t="s">
         <v>8</v>
       </c>
@@ -6876,7 +6876,7 @@
         <v>0.10891297933424089</v>
       </c>
     </row>
-    <row r="41" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="30" t="s">
         <v>8</v>
       </c>
@@ -7001,7 +7001,7 @@
         <v>0.55828955953503578</v>
       </c>
     </row>
-    <row r="42" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="30" t="s">
         <v>8</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>0.53562056641812317</v>
       </c>
     </row>
-    <row r="43" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="30" t="s">
         <v>8</v>
       </c>
@@ -7251,7 +7251,7 @@
         <v>0.3308293136222733</v>
       </c>
     </row>
-    <row r="44" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="30" t="s">
         <v>8</v>
       </c>
@@ -7376,7 +7376,7 @@
         <v>2.3563643081164449</v>
       </c>
     </row>
-    <row r="45" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="30" t="s">
         <v>8</v>
       </c>
@@ -7501,7 +7501,7 @@
         <v>0.3096676051461088</v>
       </c>
     </row>
-    <row r="46" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="30" t="s">
         <v>8</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>2.8044446154538938</v>
       </c>
     </row>
-    <row r="47" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="30" t="s">
         <v>8</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>0.48962516783660348</v>
       </c>
     </row>
-    <row r="48" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="30" t="s">
         <v>8</v>
       </c>
@@ -7876,7 +7876,7 @@
         <v>5.7639777025201941E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="30" t="s">
         <v>8</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>3.8619398403142949E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="30" t="s">
         <v>8</v>
       </c>
@@ -8126,7 +8126,7 @@
         <v>6.5551550140085998E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="30" t="s">
         <v>8</v>
       </c>
@@ -8251,7 +8251,7 @@
         <v>5.425717717790729E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:41" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:41" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="68" t="s">
         <v>8</v>
       </c>
@@ -8376,7 +8376,7 @@
         <v>3.5824311010091768E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="75" t="s">
         <v>8</v>
       </c>
@@ -8501,7 +8501,7 @@
         <v>4.4290205807614662E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="79" t="s">
         <v>8</v>
       </c>
@@ -8626,7 +8626,7 @@
         <v>6.3423574716504186E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="81" t="s">
         <v>8</v>
       </c>
@@ -8751,7 +8751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="79" t="s">
         <v>8</v>
       </c>
@@ -8876,7 +8876,7 @@
         <v>0.13075886040993689</v>
       </c>
     </row>
-    <row r="57" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="79" t="s">
         <v>8</v>
       </c>
@@ -9001,7 +9001,7 @@
         <v>3.543216464609172E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="79" t="s">
         <v>8</v>
       </c>
@@ -9126,7 +9126,7 @@
         <v>1.771608232304586E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="79" t="s">
         <v>8</v>
       </c>
@@ -9251,7 +9251,7 @@
         <v>7.8143867518722987E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="79" t="s">
         <v>8</v>
       </c>
@@ -9376,7 +9376,7 @@
         <v>0.87930585715619991</v>
       </c>
     </row>
-    <row r="61" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="79" t="s">
         <v>8</v>
       </c>
@@ -9501,7 +9501,7 @@
         <v>2.4044072051932282E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="79" t="s">
         <v>8</v>
       </c>
@@ -9626,7 +9626,7 @@
         <v>0.1559015244428035</v>
       </c>
     </row>
-    <row r="63" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="79" t="s">
         <v>8</v>
       </c>
@@ -9751,7 +9751,7 @@
         <v>0.51376638736832991</v>
       </c>
     </row>
-    <row r="64" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="79" t="s">
         <v>8</v>
       </c>
@@ -9876,7 +9876,7 @@
         <v>1.792760992344606E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="79" t="s">
         <v>8</v>
       </c>
@@ -10001,7 +10001,7 @@
         <v>6.418084352593692E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="79" t="s">
         <v>8</v>
       </c>
@@ -10126,7 +10126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="79" t="s">
         <v>8</v>
       </c>
@@ -10251,7 +10251,7 @@
         <v>0.13232010332297073</v>
       </c>
     </row>
-    <row r="68" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="79" t="s">
         <v>8</v>
       </c>
@@ -10376,7 +10376,7 @@
         <v>0.12549326946412248</v>
       </c>
     </row>
-    <row r="69" spans="1:41" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:41" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="86" t="s">
         <v>8</v>
       </c>
@@ -10501,7 +10501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>8</v>
       </c>
@@ -10626,7 +10626,7 @@
         <v>7.6296369378360556</v>
       </c>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>8</v>
       </c>
@@ -10751,7 +10751,7 @@
         <v>2.2652999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
         <v>8</v>
       </c>
@@ -10876,7 +10876,7 @@
         <v>12.277200000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A73" s="39" t="s">
         <v>8</v>
       </c>
@@ -10905,7 +10905,7 @@
         <v>59.785899999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A74" s="39" t="s">
         <v>124</v>
       </c>
@@ -10934,7 +10934,7 @@
         <v>0.38750000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A75" s="39" t="s">
         <v>124</v>
       </c>
@@ -10963,7 +10963,7 @@
         <v>0.38750000000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A76" s="39" t="s">
         <v>124</v>
       </c>
@@ -10992,7 +10992,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
         <v>8</v>
       </c>
@@ -11021,7 +11021,7 @@
         <v>28.942299999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A78" s="39" t="s">
         <v>124</v>
       </c>
@@ -11050,7 +11050,7 @@
         <v>6.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A79" s="39" t="s">
         <v>124</v>
       </c>
@@ -11079,7 +11079,7 @@
         <v>0.33529999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A80" s="39" t="s">
         <v>124</v>
       </c>
@@ -11108,7 +11108,7 @@
         <v>0.65800000000000003</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="39" t="s">
         <v>124</v>
       </c>
@@ -11137,7 +11137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="39" t="s">
         <v>124</v>
       </c>
@@ -11166,7 +11166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="39" t="s">
         <v>8</v>
       </c>
@@ -11195,7 +11195,7 @@
         <v>14.555999999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="39" t="s">
         <v>124</v>
       </c>
@@ -11224,7 +11224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="39" t="s">
         <v>8</v>
       </c>
@@ -11253,7 +11253,7 @@
         <v>12.510999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="39" t="s">
         <v>124</v>
       </c>
@@ -11282,7 +11282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="39" t="s">
         <v>124</v>
       </c>
@@ -11311,7 +11311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="39" t="s">
         <v>8</v>
       </c>
@@ -11340,7 +11340,7 @@
         <v>15.461</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="39" t="s">
         <v>124</v>
       </c>
@@ -11369,7 +11369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="39" t="s">
         <v>8</v>
       </c>
@@ -11407,6 +11407,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -11415,7 +11425,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -11646,29 +11656,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ED672C9-E834-4E4B-BB43-E87E9628BAF2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{124352EC-5983-47FF-B2F1-21582D939B66}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EFBB33F-3B30-4D18-BAAC-D5F71240E8ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11677,4 +11665,31 @@
     <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ED672C9-E834-4E4B-BB43-E87E9628BAF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{124352EC-5983-47FF-B2F1-21582D939B66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correct Demand and Parametrization excels about timeslices
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Outputs/A-O_Demand.xlsx
+++ b/t1_confection/A1_Outputs/A-O_Demand.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t1_confection\A1_Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752F78AE-F444-40B3-AFEF-49DF7BD35389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E3CFC1-46D8-4E80-8AAC-143992544F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="2490" windowWidth="21630" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Timeslices" sheetId="3" r:id="rId1"/>
-    <sheet name="Demand_Projection" sheetId="1" r:id="rId2"/>
+    <sheet name="Demand_Projection" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -352,7 +351,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="166">
   <si>
     <t>Demand/Share</t>
   </si>
@@ -850,15 +849,6 @@
   </si>
   <si>
     <t>Transport Demand non motorized reductions</t>
-  </si>
-  <si>
-    <t>Timeslice</t>
-  </si>
-  <si>
-    <t>DRY</t>
-  </si>
-  <si>
-    <t>RAIN</t>
   </si>
 </sst>
 </file>
@@ -1396,7 +1386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1540,7 +1530,6 @@
     <xf numFmtId="166" fontId="6" fillId="13" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1865,680 +1854,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037C0E4B-223C-493A-AA95-0D314598A9DF}">
-  <dimension ref="A1:AP5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
-        <v>166</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="K1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="M1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="N1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="O1" s="1">
-        <v>2023</v>
-      </c>
-      <c r="P1" s="1">
-        <v>2024</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>2025</v>
-      </c>
-      <c r="R1" s="1">
-        <v>2026</v>
-      </c>
-      <c r="S1" s="1">
-        <v>2027</v>
-      </c>
-      <c r="T1" s="1">
-        <v>2028</v>
-      </c>
-      <c r="U1" s="1">
-        <v>2029</v>
-      </c>
-      <c r="V1" s="1">
-        <v>2030</v>
-      </c>
-      <c r="W1" s="1">
-        <v>2031</v>
-      </c>
-      <c r="X1" s="1">
-        <v>2032</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>2033</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>2034</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>2035</v>
-      </c>
-      <c r="AB1" s="1">
-        <v>2036</v>
-      </c>
-      <c r="AC1" s="1">
-        <v>2037</v>
-      </c>
-      <c r="AD1" s="1">
-        <v>2038</v>
-      </c>
-      <c r="AE1" s="1">
-        <v>2039</v>
-      </c>
-      <c r="AF1" s="1">
-        <v>2040</v>
-      </c>
-      <c r="AG1" s="1">
-        <v>2041</v>
-      </c>
-      <c r="AH1" s="1">
-        <v>2042</v>
-      </c>
-      <c r="AI1" s="1">
-        <v>2043</v>
-      </c>
-      <c r="AJ1" s="1">
-        <v>2044</v>
-      </c>
-      <c r="AK1" s="1">
-        <v>2045</v>
-      </c>
-      <c r="AL1" s="1">
-        <v>2046</v>
-      </c>
-      <c r="AM1" s="1">
-        <v>2047</v>
-      </c>
-      <c r="AN1" s="1">
-        <v>2048</v>
-      </c>
-      <c r="AO1" s="1">
-        <v>2049</v>
-      </c>
-      <c r="AP1" s="1">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="2" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1.130436</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1.3405151997302078</v>
-      </c>
-      <c r="L2" s="2">
-        <v>1.155981494838745</v>
-      </c>
-      <c r="M2" s="2">
-        <v>1.3158819494067027</v>
-      </c>
-      <c r="N2" s="20">
-        <v>1.228027468725523</v>
-      </c>
-      <c r="O2" s="20">
-        <v>1.2225466516920374</v>
-      </c>
-      <c r="P2" s="20">
-        <v>1.2642991758160602</v>
-      </c>
-      <c r="Q2" s="20">
-        <v>1.3061603371669015</v>
-      </c>
-      <c r="R2" s="20">
-        <v>1.3457029459936605</v>
-      </c>
-      <c r="S2" s="20">
-        <v>1.385820995226948</v>
-      </c>
-      <c r="T2" s="20">
-        <v>1.4283570465266955</v>
-      </c>
-      <c r="U2" s="20">
-        <v>1.4693026793705557</v>
-      </c>
-      <c r="V2" s="20">
-        <v>1.5100626733919791</v>
-      </c>
-      <c r="W2" s="20">
-        <v>1.5470140015439409</v>
-      </c>
-      <c r="X2" s="20">
-        <v>1.5846567014175537</v>
-      </c>
-      <c r="Y2" s="20">
-        <v>1.6229997712220672</v>
-      </c>
-      <c r="Z2" s="20">
-        <v>1.6620522756006084</v>
-      </c>
-      <c r="AA2" s="20">
-        <v>1.70182334575065</v>
-      </c>
-      <c r="AB2" s="20">
-        <v>1.7353881862675751</v>
-      </c>
-      <c r="AC2" s="20">
-        <v>1.7694597550384985</v>
-      </c>
-      <c r="AD2" s="20">
-        <v>1.804043379247714</v>
-      </c>
-      <c r="AE2" s="20">
-        <v>1.8391444178829401</v>
-      </c>
-      <c r="AF2" s="20">
-        <v>1.8747682617819925</v>
-      </c>
-      <c r="AG2" s="20">
-        <v>1.9037214287348594</v>
-      </c>
-      <c r="AH2" s="20">
-        <v>1.9330171998608836</v>
-      </c>
-      <c r="AI2" s="20">
-        <v>1.9626584009867136</v>
-      </c>
-      <c r="AJ2" s="20">
-        <v>1.9926478711876765</v>
-      </c>
-      <c r="AK2" s="20">
-        <v>2.0229884628030699</v>
-      </c>
-      <c r="AL2" s="20">
-        <v>2.0465590535637337</v>
-      </c>
-      <c r="AM2" s="20">
-        <v>2.0703402523753147</v>
-      </c>
-      <c r="AN2" s="20">
-        <v>2.0943333720806838</v>
-      </c>
-      <c r="AO2" s="20">
-        <v>2.1185397301785733</v>
-      </c>
-      <c r="AP2" s="20">
-        <v>2.1429606488276343</v>
-      </c>
-    </row>
-    <row r="3" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1.130436</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1.3405151997302078</v>
-      </c>
-      <c r="L3" s="2">
-        <v>1.155981494838745</v>
-      </c>
-      <c r="M3" s="2">
-        <v>1.3158819494067027</v>
-      </c>
-      <c r="N3" s="20">
-        <v>1.228027468725523</v>
-      </c>
-      <c r="O3" s="20">
-        <v>1.2225466516920374</v>
-      </c>
-      <c r="P3" s="20">
-        <v>1.2642991758160602</v>
-      </c>
-      <c r="Q3" s="20">
-        <v>1.3061603371669015</v>
-      </c>
-      <c r="R3" s="20">
-        <v>1.3457029459936605</v>
-      </c>
-      <c r="S3" s="20">
-        <v>1.385820995226948</v>
-      </c>
-      <c r="T3" s="20">
-        <v>1.4283570465266955</v>
-      </c>
-      <c r="U3" s="20">
-        <v>1.4693026793705557</v>
-      </c>
-      <c r="V3" s="20">
-        <v>1.5100626733919791</v>
-      </c>
-      <c r="W3" s="20">
-        <v>1.5470140015439409</v>
-      </c>
-      <c r="X3" s="20">
-        <v>1.5846567014175537</v>
-      </c>
-      <c r="Y3" s="20">
-        <v>1.6229997712220672</v>
-      </c>
-      <c r="Z3" s="20">
-        <v>1.6620522756006084</v>
-      </c>
-      <c r="AA3" s="20">
-        <v>1.70182334575065</v>
-      </c>
-      <c r="AB3" s="20">
-        <v>1.7353881862675751</v>
-      </c>
-      <c r="AC3" s="20">
-        <v>1.7694597550384985</v>
-      </c>
-      <c r="AD3" s="20">
-        <v>1.804043379247714</v>
-      </c>
-      <c r="AE3" s="20">
-        <v>1.8391444178829401</v>
-      </c>
-      <c r="AF3" s="20">
-        <v>1.8747682617819925</v>
-      </c>
-      <c r="AG3" s="20">
-        <v>1.9037214287348594</v>
-      </c>
-      <c r="AH3" s="20">
-        <v>1.9330171998608836</v>
-      </c>
-      <c r="AI3" s="20">
-        <v>1.9626584009867136</v>
-      </c>
-      <c r="AJ3" s="20">
-        <v>1.9926478711876765</v>
-      </c>
-      <c r="AK3" s="20">
-        <v>2.0229884628030699</v>
-      </c>
-      <c r="AL3" s="20">
-        <v>2.0465590535637337</v>
-      </c>
-      <c r="AM3" s="20">
-        <v>2.0703402523753147</v>
-      </c>
-      <c r="AN3" s="20">
-        <v>2.0943333720806838</v>
-      </c>
-      <c r="AO3" s="20">
-        <v>2.1185397301785733</v>
-      </c>
-      <c r="AP3" s="20">
-        <v>2.1429606488276343</v>
-      </c>
-    </row>
-    <row r="4" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1.130436</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1.3405151997302078</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1.155981494838745</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1.3158819494067027</v>
-      </c>
-      <c r="N4" s="20">
-        <v>1.228027468725523</v>
-      </c>
-      <c r="O4" s="20">
-        <v>1.2225466516920374</v>
-      </c>
-      <c r="P4" s="20">
-        <v>1.2642991758160602</v>
-      </c>
-      <c r="Q4" s="20">
-        <v>1.3061603371669015</v>
-      </c>
-      <c r="R4" s="20">
-        <v>1.3457029459936605</v>
-      </c>
-      <c r="S4" s="20">
-        <v>1.385820995226948</v>
-      </c>
-      <c r="T4" s="20">
-        <v>1.4283570465266955</v>
-      </c>
-      <c r="U4" s="20">
-        <v>1.4693026793705557</v>
-      </c>
-      <c r="V4" s="20">
-        <v>1.5100626733919791</v>
-      </c>
-      <c r="W4" s="20">
-        <v>1.5470140015439409</v>
-      </c>
-      <c r="X4" s="20">
-        <v>1.5846567014175537</v>
-      </c>
-      <c r="Y4" s="20">
-        <v>1.6229997712220672</v>
-      </c>
-      <c r="Z4" s="20">
-        <v>1.6620522756006084</v>
-      </c>
-      <c r="AA4" s="20">
-        <v>1.70182334575065</v>
-      </c>
-      <c r="AB4" s="20">
-        <v>1.7353881862675751</v>
-      </c>
-      <c r="AC4" s="20">
-        <v>1.7694597550384985</v>
-      </c>
-      <c r="AD4" s="20">
-        <v>1.804043379247714</v>
-      </c>
-      <c r="AE4" s="20">
-        <v>1.8391444178829401</v>
-      </c>
-      <c r="AF4" s="20">
-        <v>1.8747682617819925</v>
-      </c>
-      <c r="AG4" s="20">
-        <v>1.9037214287348594</v>
-      </c>
-      <c r="AH4" s="20">
-        <v>1.9330171998608836</v>
-      </c>
-      <c r="AI4" s="20">
-        <v>1.9626584009867136</v>
-      </c>
-      <c r="AJ4" s="20">
-        <v>1.9926478711876765</v>
-      </c>
-      <c r="AK4" s="20">
-        <v>2.0229884628030699</v>
-      </c>
-      <c r="AL4" s="20">
-        <v>2.0465590535637337</v>
-      </c>
-      <c r="AM4" s="20">
-        <v>2.0703402523753147</v>
-      </c>
-      <c r="AN4" s="20">
-        <v>2.0943333720806838</v>
-      </c>
-      <c r="AO4" s="20">
-        <v>2.1185397301785733</v>
-      </c>
-      <c r="AP4" s="20">
-        <v>2.1429606488276343</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1.130436</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1.3405151997302078</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1.155981494838745</v>
-      </c>
-      <c r="M5" s="2">
-        <v>1.3158819494067027</v>
-      </c>
-      <c r="N5" s="20">
-        <v>1.228027468725523</v>
-      </c>
-      <c r="O5" s="20">
-        <v>1.2225466516920374</v>
-      </c>
-      <c r="P5" s="20">
-        <v>1.2642991758160602</v>
-      </c>
-      <c r="Q5" s="20">
-        <v>1.3061603371669015</v>
-      </c>
-      <c r="R5" s="20">
-        <v>1.3457029459936605</v>
-      </c>
-      <c r="S5" s="20">
-        <v>1.385820995226948</v>
-      </c>
-      <c r="T5" s="20">
-        <v>1.4283570465266955</v>
-      </c>
-      <c r="U5" s="20">
-        <v>1.4693026793705557</v>
-      </c>
-      <c r="V5" s="20">
-        <v>1.5100626733919791</v>
-      </c>
-      <c r="W5" s="20">
-        <v>1.5470140015439409</v>
-      </c>
-      <c r="X5" s="20">
-        <v>1.5846567014175537</v>
-      </c>
-      <c r="Y5" s="20">
-        <v>1.6229997712220672</v>
-      </c>
-      <c r="Z5" s="20">
-        <v>1.6620522756006084</v>
-      </c>
-      <c r="AA5" s="20">
-        <v>1.70182334575065</v>
-      </c>
-      <c r="AB5" s="20">
-        <v>1.7353881862675751</v>
-      </c>
-      <c r="AC5" s="20">
-        <v>1.7694597550384985</v>
-      </c>
-      <c r="AD5" s="20">
-        <v>1.804043379247714</v>
-      </c>
-      <c r="AE5" s="20">
-        <v>1.8391444178829401</v>
-      </c>
-      <c r="AF5" s="20">
-        <v>1.8747682617819925</v>
-      </c>
-      <c r="AG5" s="20">
-        <v>1.9037214287348594</v>
-      </c>
-      <c r="AH5" s="20">
-        <v>1.9330171998608836</v>
-      </c>
-      <c r="AI5" s="20">
-        <v>1.9626584009867136</v>
-      </c>
-      <c r="AJ5" s="20">
-        <v>1.9926478711876765</v>
-      </c>
-      <c r="AK5" s="20">
-        <v>2.0229884628030699</v>
-      </c>
-      <c r="AL5" s="20">
-        <v>2.0465590535637337</v>
-      </c>
-      <c r="AM5" s="20">
-        <v>2.0703402523753147</v>
-      </c>
-      <c r="AN5" s="20">
-        <v>2.0943333720806838</v>
-      </c>
-      <c r="AO5" s="20">
-        <v>2.1185397301785733</v>
-      </c>
-      <c r="AP5" s="20">
-        <v>2.1429606488276343</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO90"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -12088,6 +11407,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -12318,26 +11656,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EFBB33F-3B30-4D18-BAAC-D5F71240E8ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ED672C9-E834-4E4B-BB43-E87E9628BAF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{124352EC-5983-47FF-B2F1-21582D939B66}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12354,23 +11692,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ED672C9-E834-4E4B-BB43-E87E9628BAF2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EFBB33F-3B30-4D18-BAAC-D5F71240E8ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
-    <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>